<commit_message>
ajout de la vérification des cases à cocher et de la coloration des lignes du fichier excel
</commit_message>
<xml_diff>
--- a/media/donnees_extraites.xlsx
+++ b/media/donnees_extraites.xlsx
@@ -29,12 +29,24 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00CFFFB3"/>
+        <bgColor rgb="00CFFFB3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF4B3E"/>
+        <bgColor rgb="00FF4B3E"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -55,11 +67,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +439,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Z2"/>
+  <dimension ref="A1:AC3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,7 +455,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Nom du bateau</t>
+          <t>Nom de course</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -451,249 +465,226 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Skipper</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Responsable du bateau pour les contrôles</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Téléphone</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>MMSI</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>N° de série</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>prochaine révision</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Marque gilet skipper</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Couleur gilet skipper</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Nom inscrit sur le gilet skipper</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Marque gilet Spare</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Couleur gilet Spare</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Nom inscrit sur le gilet Spare</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Balise Personelle AIS</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>2ème Balise Personelle AIS</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>PLB</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>2ème PLB</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Numéro combinaison de survie</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>Couleur combinaison de survie</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>Marque combinaison de survie</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Indicatif VHF</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>Numéro Iridium</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>N° EPIRB</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>Date révision EPIRB</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
           <t>Soussigné</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Contacts téléphoniques</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>MMSI</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Téléphone satellitaire</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>EPIRB</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>NomPrénom1</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Balise AIS1</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Balise PLB1</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>NomPrénom2</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Balise AIS2</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>Balise PLB2</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>NomPrénom3</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>Balise AIS3</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>Balise PLB3</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>NomPrénom4</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>Balise AIS4</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>Balise PLB4</t>
-        </is>
-      </c>
-      <c r="U1" s="1" t="inlineStr">
-        <is>
-          <t>NomPrénom5</t>
-        </is>
-      </c>
-      <c r="V1" s="1" t="inlineStr">
-        <is>
-          <t>Balise AIS5</t>
-        </is>
-      </c>
-      <c r="W1" s="1" t="inlineStr">
-        <is>
-          <t>Balise PLB5</t>
-        </is>
-      </c>
-      <c r="X1" s="1" t="inlineStr">
-        <is>
-          <t>NomPrénom6</t>
-        </is>
-      </c>
-      <c r="Y1" s="1" t="inlineStr">
-        <is>
-          <t>Balise AIS6</t>
-        </is>
-      </c>
-      <c r="Z1" s="1" t="inlineStr">
-        <is>
-          <t>Balise PLB6</t>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>Controle</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Inconnu</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Inconnu</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Inconnu</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Inconnu</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Inconnu</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Inconnu</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Inconnu</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>Inconnu</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>Inconnu</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>Inconnu</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>Inconnu</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>Inconnu</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>Inconnu</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>Inconnu</t>
-        </is>
-      </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>Inconnu</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>Inconnu</t>
-        </is>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>Inconnu</t>
-        </is>
-      </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>Inconnu</t>
-        </is>
-      </c>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>Inconnu</t>
-        </is>
-      </c>
-      <c r="U2" t="inlineStr">
-        <is>
-          <t>Inconnu</t>
-        </is>
-      </c>
-      <c r="V2" t="inlineStr">
-        <is>
-          <t>Inconnu</t>
-        </is>
-      </c>
-      <c r="W2" t="inlineStr">
-        <is>
-          <t>Inconnu</t>
-        </is>
-      </c>
-      <c r="X2" t="inlineStr">
-        <is>
-          <t>Inconnu</t>
-        </is>
-      </c>
-      <c r="Y2" t="inlineStr">
-        <is>
-          <t>Inconnu</t>
-        </is>
-      </c>
-      <c r="Z2" t="inlineStr">
-        <is>
-          <t>Inconnu</t>
+      <c r="A2" s="2" t="inlineStr"/>
+      <c r="B2" s="2" t="inlineStr"/>
+      <c r="C2" s="2" t="inlineStr"/>
+      <c r="D2" s="2" t="inlineStr"/>
+      <c r="E2" s="2" t="inlineStr"/>
+      <c r="F2" s="2" t="inlineStr"/>
+      <c r="G2" s="2" t="inlineStr"/>
+      <c r="H2" s="2" t="inlineStr"/>
+      <c r="I2" s="2" t="inlineStr"/>
+      <c r="J2" s="2" t="inlineStr"/>
+      <c r="K2" s="2" t="inlineStr">
+        <is>
+          <t>Orange</t>
+        </is>
+      </c>
+      <c r="L2" s="2" t="inlineStr"/>
+      <c r="M2" s="2" t="inlineStr"/>
+      <c r="N2" s="2" t="inlineStr">
+        <is>
+          <t>Orange</t>
+        </is>
+      </c>
+      <c r="O2" s="2" t="inlineStr"/>
+      <c r="P2" s="2" t="inlineStr"/>
+      <c r="Q2" s="2" t="inlineStr"/>
+      <c r="R2" s="2" t="inlineStr"/>
+      <c r="S2" s="2" t="inlineStr"/>
+      <c r="T2" s="2" t="inlineStr"/>
+      <c r="U2" s="2" t="inlineStr"/>
+      <c r="V2" s="2" t="inlineStr"/>
+      <c r="W2" s="2" t="inlineStr"/>
+      <c r="X2" s="2" t="inlineStr">
+        <is>
+          <t>00</t>
+        </is>
+      </c>
+      <c r="Y2" s="2" t="inlineStr"/>
+      <c r="Z2" s="2" t="inlineStr"/>
+      <c r="AA2" s="2" t="inlineStr"/>
+      <c r="AB2" s="2" t="inlineStr"/>
+      <c r="AC2" s="2" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="inlineStr"/>
+      <c r="B3" s="3" t="inlineStr"/>
+      <c r="C3" s="3" t="inlineStr"/>
+      <c r="D3" s="3" t="inlineStr"/>
+      <c r="E3" s="3" t="inlineStr"/>
+      <c r="F3" s="3" t="inlineStr"/>
+      <c r="G3" s="3" t="inlineStr"/>
+      <c r="H3" s="3" t="inlineStr"/>
+      <c r="I3" s="3" t="inlineStr"/>
+      <c r="J3" s="3" t="inlineStr"/>
+      <c r="K3" s="3" t="inlineStr">
+        <is>
+          <t>Orange</t>
+        </is>
+      </c>
+      <c r="L3" s="3" t="inlineStr"/>
+      <c r="M3" s="3" t="inlineStr"/>
+      <c r="N3" s="3" t="inlineStr">
+        <is>
+          <t>Orange</t>
+        </is>
+      </c>
+      <c r="O3" s="3" t="inlineStr"/>
+      <c r="P3" s="3" t="inlineStr"/>
+      <c r="Q3" s="3" t="inlineStr"/>
+      <c r="R3" s="3" t="inlineStr"/>
+      <c r="S3" s="3" t="inlineStr"/>
+      <c r="T3" s="3" t="inlineStr"/>
+      <c r="U3" s="3" t="inlineStr"/>
+      <c r="V3" s="3" t="inlineStr"/>
+      <c r="W3" s="3" t="inlineStr"/>
+      <c r="X3" s="3" t="inlineStr">
+        <is>
+          <t>00</t>
+        </is>
+      </c>
+      <c r="Y3" s="3" t="inlineStr"/>
+      <c r="Z3" s="3" t="inlineStr"/>
+      <c r="AA3" s="3" t="inlineStr"/>
+      <c r="AB3" s="3" t="inlineStr"/>
+      <c r="AC3" s="3" t="inlineStr">
+        <is>
+          <t>Non OK</t>
         </is>
       </c>
     </row>

</xml_diff>